<commit_message>
updated results and optimized random some random forest parameters
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>distance</t>
   </si>
@@ -37,14 +37,34 @@
   </si>
   <si>
     <t>error if we remove "day"</t>
+  </si>
+  <si>
+    <t>error if we remove "month"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max depth </t>
+  </si>
+  <si>
+    <t>n estimators</t>
+  </si>
+  <si>
+    <t>REMOVE WEEKDAY AND MONTH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,37 +105,75 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -456,9 +514,10 @@
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:7" ht="45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,23 +530,55 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>69.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>68.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
@@ -500,8 +591,11 @@
       <c r="D5">
         <v>69.099999999999994</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>64.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1</v>
       </c>
@@ -515,7 +609,7 @@
         <v>69.349999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -529,7 +623,7 @@
         <v>69.78</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>0.25</v>
       </c>
@@ -543,7 +637,7 @@
         <v>70.17</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>0.125</v>
       </c>
@@ -555,6 +649,177 @@
       </c>
       <c r="D9" s="1">
         <v>70.540000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>75.83</v>
+      </c>
+      <c r="D13" s="3">
+        <v>58.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1">
+        <v>71.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>66.569999999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>65.209999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3">
+        <v>64.83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>65.12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>65.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>67.069999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>67.180000000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>66.290000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>65.290000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>64.77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>80</v>
+      </c>
+      <c r="C25">
+        <v>64.39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>160</v>
+      </c>
+      <c r="C26">
+        <v>64.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some more features individually. 911_w_features is almost ready. Just need to append the auto_thefts onto it (it's running now). error down to 58.37
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23080" yWindow="1100" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="14100" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
-  <si>
-    <t>distance</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>classifier</t>
   </si>
@@ -49,6 +46,21 @@
   </si>
   <si>
     <t>REMOVE WEEKDAY AND MONTH</t>
+  </si>
+  <si>
+    <t>REMOVE WEEKDAY AND MONTH AND HOUR</t>
+  </si>
+  <si>
+    <t>PARKS distance</t>
+  </si>
+  <si>
+    <t>PRIVATE SCHOOLS dist</t>
+  </si>
+  <si>
+    <t>TRAFFIC CAMERAS dist</t>
+  </si>
+  <si>
+    <t>IF WE DROP PRIVATE</t>
   </si>
 </sst>
 </file>
@@ -105,8 +117,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -145,7 +163,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -160,6 +178,9 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -174,6 +195,9 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -515,78 +539,157 @@
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" ht="45">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
       <c r="D2">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>58.64</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>58.54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
       <c r="D3">
         <v>69.98</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>58.53</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3">
+        <v>58.37</v>
+      </c>
+      <c r="N3">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
       <c r="D4">
         <v>68.92</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>58.52</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="4">
+        <v>58.51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
       </c>
       <c r="D5">
         <v>69.099999999999994</v>
@@ -594,13 +697,31 @@
       <c r="E5">
         <v>64.42</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>58.63</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>58.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>70.709999999999994</v>
@@ -608,13 +729,31 @@
       <c r="D6">
         <v>69.349999999999994</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>58.63</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>0.5</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>71.44</v>
@@ -622,13 +761,31 @@
       <c r="D7">
         <v>69.78</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7">
+        <v>0.25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>59.01</v>
+      </c>
+      <c r="K7">
+        <v>0.25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>58.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>0.25</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>71.92</v>
@@ -637,12 +794,12 @@
         <v>70.17</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>0.125</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>72.77</v>
@@ -651,21 +808,24 @@
         <v>70.540000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:14" ht="75">
       <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>2</v>
       </c>
@@ -678,8 +838,11 @@
       <c r="D13" s="3">
         <v>58.67</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="E13">
+        <v>59.11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>5</v>
       </c>
@@ -690,7 +853,7 @@
         <v>71.67</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>10</v>
       </c>
@@ -701,7 +864,7 @@
         <v>66.569999999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
911_w_features.csv is the features. The ones I optimized distance for are at the optimal distance. 911_w_features_0.5.csv is the features when distance is always 0.5
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="14100" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="32840" yWindow="-20" windowWidth="18360" windowHeight="28400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="20">
   <si>
     <t>classifier</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>IF WE DROP PRIVATE</t>
+  </si>
+  <si>
+    <t>FISHING PIERS dist</t>
+  </si>
+  <si>
+    <t>MOVIE THEATERS</t>
+  </si>
+  <si>
+    <t>Fishing piers = 2</t>
+  </si>
+  <si>
+    <t>SVC (linear)</t>
+  </si>
+  <si>
+    <t>SVC(rbf) 100 folds</t>
+  </si>
+  <si>
+    <t>WITH ALL FEATURES</t>
   </si>
 </sst>
 </file>
@@ -117,8 +135,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -181,6 +209,11 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -198,6 +231,11 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,23 +565,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:22" ht="45">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -581,8 +621,26 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>16</v>
       </c>
@@ -613,8 +671,26 @@
       <c r="M2">
         <v>58.54</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>58.41</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>58.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>8</v>
       </c>
@@ -648,9 +724,27 @@
       <c r="N3">
         <v>58.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4">
+      <c r="P3" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="4">
+        <v>58.45</v>
+      </c>
+      <c r="T3" s="4">
+        <v>4</v>
+      </c>
+      <c r="U3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>58.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="3">
         <v>4</v>
       </c>
       <c r="B4" t="s">
@@ -659,7 +753,7 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>68.92</v>
       </c>
       <c r="G4" s="3">
@@ -680,8 +774,26 @@
       <c r="M4" s="4">
         <v>58.51</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="P4" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="3">
+        <v>58.31</v>
+      </c>
+      <c r="T4" s="4">
+        <v>2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>58.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>2</v>
       </c>
@@ -715,8 +827,26 @@
       <c r="M5">
         <v>58.46</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>58.35</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>58.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>1</v>
       </c>
@@ -747,8 +877,26 @@
       <c r="M6">
         <v>58.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="P6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>58.51</v>
+      </c>
+      <c r="T6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="U6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>58.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -779,8 +927,26 @@
       <c r="M7">
         <v>58.52</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="P7">
+        <v>0.25</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>58.53</v>
+      </c>
+      <c r="T7">
+        <v>0.25</v>
+      </c>
+      <c r="U7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7">
+        <v>58.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>0.25</v>
       </c>
@@ -794,7 +960,7 @@
         <v>70.17</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>0.125</v>
       </c>
@@ -808,7 +974,7 @@
         <v>70.540000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="75">
+    <row r="12" spans="1:22" ht="75">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -824,8 +990,20 @@
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="P12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>2</v>
       </c>
@@ -841,8 +1019,17 @@
       <c r="E13">
         <v>59.11</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="Q13" s="3">
+        <v>58.31</v>
+      </c>
+      <c r="R13">
+        <v>77.48</v>
+      </c>
+      <c r="S13">
+        <v>68.55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>5</v>
       </c>
@@ -852,8 +1039,11 @@
       <c r="C14" s="1">
         <v>71.67</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="S14">
+        <v>67.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>10</v>
       </c>
@@ -863,8 +1053,11 @@
       <c r="C15">
         <v>66.569999999999993</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="S15">
+        <v>67.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>12</v>
       </c>
@@ -874,8 +1067,11 @@
       <c r="C16">
         <v>65.209999999999994</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="S16">
+        <v>67.34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -886,7 +1082,7 @@
         <v>64.83</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -897,7 +1093,7 @@
         <v>65.12</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="4">
         <v>20</v>
       </c>
@@ -908,7 +1104,7 @@
         <v>65.86</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>30</v>
       </c>
@@ -919,7 +1115,7 @@
         <v>67.069999999999993</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>40</v>
       </c>
@@ -930,7 +1126,7 @@
         <v>67.180000000000007</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>15</v>
       </c>
@@ -941,7 +1137,7 @@
         <v>66.290000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>15</v>
       </c>
@@ -952,7 +1148,7 @@
         <v>65.290000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>15</v>
       </c>
@@ -963,18 +1159,18 @@
         <v>64.77</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>15</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>80</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>64.39</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>15</v>
       </c>
@@ -983,6 +1179,25 @@
       </c>
       <c r="C26">
         <v>64.48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>80</v>
+      </c>
+      <c r="C29" s="3">
+        <v>58.2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IDK. I updated the excel a little
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32840" yWindow="-20" windowWidth="18360" windowHeight="28400" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,8 +135,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -191,7 +251,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="105">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -214,6 +274,36 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -236,6 +326,36 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -990,6 +1110,7 @@
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K12" s="4"/>
       <c r="P12" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>